<commit_message>
converted successfully. tested with only 2 items from each category.
</commit_message>
<xml_diff>
--- a/Chaldal_scraper/scrapped_data/Chaldaal_rawdata_v1.1.xlsx
+++ b/Chaldal_scraper/scrapped_data/Chaldaal_rawdata_v1.1.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="menu_urls" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="submenu_urls" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -616,4 +617,887 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Fruits &amp; Vegetables</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/fruits-vegetables</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Meat &amp; Fish</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/meat-fish</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cooking</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/cooking</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sauces &amp; Pickles</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/sauces-pickles</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Dairy &amp; Eggs</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/dairy</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Breakfast</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/breakfast</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Candy &amp; Chocolate</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/candy-chocolate</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/snacks</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Beverages</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/beverages</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Baking</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/baking-needs</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Frozen &amp; Canned</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/frozen-foods</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Diabetic Food</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/diabetic-food</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dishwashing Supplies</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/dish-wash</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Laundry</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/laundry</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Toilet Cleaners</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/toilet-cleaning</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Napkins &amp; Paper Products</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/paper-products</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pest Control</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/pest-control</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Floor &amp; Glass Cleaners</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/floor-glass-cleaners</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Cleaning Accessories</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/cleaning-accessories</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Air Fresheners</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/air-freshners</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Disposables &amp; Trash Bags</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/trash-bags</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Shoe Care</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/shoe-care</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Trash Bin &amp; Basket</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/trash-bin-basket</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Women's Care</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/female-care</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Men's Care</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/male-care</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Handwash</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/handwash</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Tissue &amp; Wipes</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/tissue-wipes</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Oral Care</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/oral-care-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Skin Care</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/skin-care-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Talcom Powder</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/talcom-powder</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Hair Color</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/hair-color</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Keto Food</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/keto-food</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Antiseptics</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/antiseptics</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Handwash &amp; Handrub</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/handwash-handrub</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Herbal &amp; Digestive Aids</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/herbal-products</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Food Supplements</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/food-supplements</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Face Masks &amp; Safety</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/face-masks-safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Family Planning</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/family-planning</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Mouthwashes, Inhaler &amp; Balm</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/mouthwashes</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Adult Diapers</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/adult-diapers</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Medical Devices</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/medical-devices</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Diapers</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/diapers</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Baby Food</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/fooding</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Baby Skincare</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/bath-skincare</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Wipes</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/wipes</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Baby Oral Care</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/baby-oral-care</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Newborn Essentials</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/newborn-essentials</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Baby Accessories</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/baby-accessories</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Feeders</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/feeders</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Kitchen Accessories</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/kitchen-accessories</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Kitchen Appliances</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/kitchen-appliances</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Lights &amp; Electrical</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/lights-electrical</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Tools &amp; Hardware</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/tools-hardware</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Basket &amp; Bucket</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/baskets-buckets</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Box &amp; Container</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/box-container</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Gardening</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/gardening</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Rack &amp; Organizer</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/rack-organizer</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Disposables</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/disposables</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Office Electronics</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/office-electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Organizers</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/organizers</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Writing &amp; Printing</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/writing</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Paper Supplies</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/paper-supplies</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>School Supplies</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/school-supplies</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Arts &amp; Crafts</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/arts-crafts</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Cat Food</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/cat-food</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Cat Litters</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/cat-litters</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Kitten Food</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/kitten-food</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Dog Food</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/dog-food</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Grooming &amp; Cleaning</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/pet-grooming-cleaning</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Bird &amp; Other Pet Food</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/bird-food</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Aquarium Fish Food</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://chaldal.com/aquarium-fish-food</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>